<commit_message>
Tools image updated (Optimica changed from devel. to Prototype)
</commit_message>
<xml_diff>
--- a/assets/images/tools.xlsx
+++ b/assets/images/tools.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\otter\_subversion\EMPHYSIS\trunk\40_Meetings\2021-02-10_ITEA-Final-Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\otter\_github\EMPHYSIS\EMPHYSIS.github.io\assets\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAC2BE2-1267-4EBA-AA98-8F9631C88934}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5563FC41-DBAC-499B-AE28-786B38408B25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="0" windowWidth="22530" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10530" yWindow="0" windowWidth="22530" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="42">
   <si>
     <t>Tool Name</t>
   </si>
@@ -318,9 +318,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFFF5050"/>
       <color rgb="FF00A151"/>
       <color rgb="FF008000"/>
+      <color rgb="FFFF5050"/>
     </mruColors>
   </colors>
   <extLst>
@@ -634,7 +634,7 @@
   <dimension ref="B1:P16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,7 +761,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="17"/>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="15" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="16"/>

</xml_diff>